<commit_message>
Add formatting to pivot example
</commit_message>
<xml_diff>
--- a/code_examples/excel_from_python/pivot.xlsx
+++ b/code_examples/excel_from_python/pivot.xlsx
@@ -65,8 +65,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -94,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,11 +615,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -738,36 +754,36 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <f>SUMIF(B2:B7, "Clothing", E2:E7)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <f>SUMIF(B2:B7, "Clothing", E2:E7)</f>
+        <f>SUMIF(B2:B7, "Stickers", E2:E7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <f>SUMIF(B2:B7, "Stickers", E2:E7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16">
         <f>SUMIF(B2:B7, "Pets", E2:E7)</f>
         <v>0</v>
       </c>

</xml_diff>